<commit_message>
fixed week 7 resources
</commit_message>
<xml_diff>
--- a/Back-End/Service_Requests.xlsx
+++ b/Back-End/Service_Requests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardo/Desktop/fcul/AW/aw-project/Back-End/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Mestrado\ApplicationWebProjectTask1\Back-End\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FAC564C-8A3F-3945-A628-5F3079D15A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884D60B8-CBF4-4C64-983D-2EA3112A2656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F2A73EE6-DCB9-4D87-8BED-ACA340A81393}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F2A73EE6-DCB9-4D87-8BED-ACA340A81393}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
-  <si>
-    <t>Market Service</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
   <si>
     <t>Product Service</t>
   </si>
@@ -71,24 +68,9 @@
     <t>GET</t>
   </si>
   <si>
-    <t>/supermarkets</t>
-  </si>
-  <si>
-    <t>/supermarkets/{supermarket_id}</t>
-  </si>
-  <si>
     <t>/supermarket/{supermarket_id}</t>
   </si>
   <si>
-    <t>/products/supermarket/{supermarket_id}</t>
-  </si>
-  <si>
-    <t>/products/{product_id}/supermarket/{supermarket_id}/</t>
-  </si>
-  <si>
-    <t>/products/{qr_code_id}</t>
-  </si>
-  <si>
     <t>/news</t>
   </si>
   <si>
@@ -101,24 +83,15 @@
     <t>POST</t>
   </si>
   <si>
-    <t>/feedback/{product_id}/value?</t>
-  </si>
-  <si>
     <t xml:space="preserve">DELETE </t>
   </si>
   <si>
-    <t>/product</t>
-  </si>
-  <si>
     <t>/supermarket</t>
   </si>
   <si>
     <t xml:space="preserve">PUT </t>
   </si>
   <si>
-    <t>/products/{id}</t>
-  </si>
-  <si>
     <t>/auth/register</t>
   </si>
   <si>
@@ -203,12 +176,6 @@
     <t>/user/{user_id}/favorites</t>
   </si>
   <si>
-    <t>/product/{product_id}</t>
-  </si>
-  <si>
-    <t>/products/{product_id}</t>
-  </si>
-  <si>
     <t>eliminar um market</t>
   </si>
   <si>
@@ -216,6 +183,27 @@
   </si>
   <si>
     <t>obter um market</t>
+  </si>
+  <si>
+    <t>Supermarket Service</t>
+  </si>
+  <si>
+    <t>/product/{product_id}/supermarket/{supermarket_id}/</t>
+  </si>
+  <si>
+    <t>/product/{qr_code_id}</t>
+  </si>
+  <si>
+    <t>/product/supermarket/{supermarket_id}</t>
+  </si>
+  <si>
+    <t>obter os produtos de um supermercado</t>
+  </si>
+  <si>
+    <t>obter o produto de um supermercado</t>
+  </si>
+  <si>
+    <t>/feedback/{product_id}/supermarket/{supermarket_id}/{value}</t>
   </si>
 </sst>
 </file>
@@ -593,380 +581,377 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D49331-9F67-49E9-A3A2-67F894DDA825}">
-  <dimension ref="E2:H30"/>
+  <dimension ref="E2:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="159" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" customWidth="1"/>
-    <col min="7" max="7" width="55.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="3" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="5:8" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E4" s="2"/>
       <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
       <c r="H4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="5:8" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E5" s="2"/>
       <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E6" s="2"/>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E7" s="2"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="H7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E8" s="2" t="s">
-        <v>1</v>
-      </c>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E8" s="2"/>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="5:8" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="H8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E9" s="2"/>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="5:8" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E10" s="2"/>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="5:8" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E11" s="2"/>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="5:8" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E12" s="2"/>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="H12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E13" s="2"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E14" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E14" s="2"/>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="5:8" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E15" s="2"/>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G15" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="5:8" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E16" s="2"/>
       <c r="F16" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E17" s="2"/>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E18" s="2"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="F18" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G18" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="H18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E19" s="2" t="s">
-        <v>3</v>
-      </c>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E20" s="2"/>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E23" s="2"/>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s">
         <v>19</v>
       </c>
-      <c r="H20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E21" s="2"/>
-      <c r="F21" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>27</v>
       </c>
-      <c r="H23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="5:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E24" s="2"/>
       <c r="F24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" t="s">
         <v>20</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>28</v>
       </c>
-      <c r="H24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="5:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E25" s="2"/>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G25" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" t="s">
         <v>29</v>
       </c>
-      <c r="H25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E26" s="2"/>
+    </row>
+    <row r="26" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E26" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="F26" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G26" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="H26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E27" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E27" s="2"/>
       <c r="F27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G27" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="5:8" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E28" s="2"/>
       <c r="F28" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="H28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="5:8" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E29" s="2"/>
       <c r="F29" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G29" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H29" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E30" s="2"/>
-      <c r="F30" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" t="s">
-        <v>53</v>
-      </c>
-      <c r="H30" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="E3:E7"/>
-    <mergeCell ref="E8:E13"/>
-    <mergeCell ref="E14:E18"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="E7:E12"/>
+    <mergeCell ref="E13:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added yaml file and fixed services table
Co-authored-by: Frederico Prazeres <fc56269@alunos.fc.ul.pt>
</commit_message>
<xml_diff>
--- a/Back-End/Service_Requests.xlsx
+++ b/Back-End/Service_Requests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Mestrado\ApplicationWebProjectTask1\Back-End\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuyu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884D60B8-CBF4-4C64-983D-2EA3112A2656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F828DA44-6D0B-4233-A099-7472FADEDB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F2A73EE6-DCB9-4D87-8BED-ACA340A81393}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F2A73EE6-DCB9-4D87-8BED-ACA340A81393}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D49331-9F67-49E9-A3A2-67F894DDA825}">
   <dimension ref="E2:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +885,7 @@
     <row r="25" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E25" s="2"/>
       <c r="F25" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G25" t="s">
         <v>21</v>

</xml_diff>